<commit_message>
Update from CTP review round 2.
</commit_message>
<xml_diff>
--- a/static/fields/tobaccoproblem_reference.xlsx
+++ b/static/fields/tobaccoproblem_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76B9FFCB-AA9E-A441-A2CC-AFEA472466A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0758F447-12F0-604E-97A3-A17FC03E5747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="760" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,18 +51,12 @@
     <t>7-digit ICSR number (no spaces).</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>submission_date</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>Date of Original Receipt to FDA.</t>
-  </si>
-  <si>
     <t>reported_product_problems</t>
   </si>
   <si>
@@ -93,13 +87,19 @@
     <t>number_health_problems</t>
   </si>
   <si>
-    <t>ystem-calculated number of Health Problems (i.e., MedDRA terms selected from a standardized list of symptoms, signs, diagnoses and outcomes) reported, displayed as a whole number, ≥0.</t>
-  </si>
-  <si>
     <t>nonuser_affected</t>
   </si>
   <si>
-    <t>Displays text reflecting the response to this optional question as “No information provided” if not answered, or Yes/No.</t>
+    <t>System-calculated number of Health Problems (i.e., MedDRA terms selected from a standardized list of symptoms, signs, diagnoses and outcomes) reported, displayed as a whole number, ≥0.</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Displays text reflecting the response to this optional question (2017 - 12/14/2018) or required question (12/15/2018 onward) as “No information provided” if not answered, or Yes/No.</t>
+  </si>
+  <si>
+    <t>Date report was received by CTP; this is the earliest date of report receipt, either to Safety Reporting Portal (SRP) or by other means</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,46 +989,46 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1036,58 +1036,58 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="57" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="65" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Round 4 of FDA review.
</commit_message>
<xml_diff>
--- a/static/fields/tobaccoproblem_reference.xlsx
+++ b/static/fields/tobaccoproblem_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0758F447-12F0-604E-97A3-A17FC03E5747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7066E9-48E2-C146-A1AC-BB4C09236DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="760" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11660" yWindow="460" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>product_type</t>
-  </si>
-  <si>
     <t>array</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Date report was received by CTP; this is the earliest date of report receipt, either to Safety Reporting Portal (SRP) or by other means</t>
+  </si>
+  <si>
+    <t>tobacco_products</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,101 +986,101 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round 5 of FDA review.
</commit_message>
<xml_diff>
--- a/static/fields/tobaccoproblem_reference.xlsx
+++ b/static/fields/tobaccoproblem_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7066E9-48E2-C146-A1AC-BB4C09236DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F6FDF-243A-BB49-B079-82CE054D2165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="460" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="460" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>7-digit ICSR number (no spaces).</t>
   </si>
   <si>
-    <t>submission_date</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -96,10 +93,13 @@
     <t>Displays text reflecting the response to this optional question (2017 - 12/14/2018) or required question (12/15/2018 onward) as “No information provided” if not answered, or Yes/No.</t>
   </si>
   <si>
-    <t>Date report was received by CTP; this is the earliest date of report receipt, either to Safety Reporting Portal (SRP) or by other means</t>
-  </si>
-  <si>
     <t>tobacco_products</t>
+  </si>
+  <si>
+    <t>date_submitted</t>
+  </si>
+  <si>
+    <t>Date report was received by CTP; this is the earliest date of report receipt, either to Safety Reporting Portal (SRP) or by other means. Date follows format: `YYYYmmdd`.</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,12 +984,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -997,90 +997,90 @@
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>